<commit_message>
Week 2: Dataloader read all files correctly, now change them to Data
</commit_message>
<xml_diff>
--- a/Data/opis_przejsc.xlsx
+++ b/Data/opis_przejsc.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Marcin\Desktop\Studia\IoT\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4C1B3054-C405-4085-BE7D-E1255D4270DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877F6039-554B-4630-AD62-BE43A9D780BD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="214" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="154">
   <si>
     <t>Lp</t>
   </si>
@@ -481,6 +481,12 @@
   </si>
   <si>
     <t>20250314121230R_pjinkim</t>
+  </si>
+  <si>
+    <t>start</t>
+  </si>
+  <si>
+    <t>stop</t>
   </si>
 </sst>
 </file>
@@ -798,10 +804,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:D71"/>
+  <dimension ref="A1:F71"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A43" workbookViewId="0">
-      <selection activeCell="I57" sqref="I57"/>
+    <sheetView tabSelected="1" topLeftCell="A15" workbookViewId="0">
+      <selection activeCell="G66" sqref="G66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -810,7 +816,7 @@
     <col min="3" max="3" width="24.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -823,8 +829,14 @@
       <c r="D1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>152</v>
+      </c>
+      <c r="F1" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -837,8 +849,14 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>20</v>
+      </c>
+      <c r="F2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -851,8 +869,14 @@
       <c r="D3" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E3">
+        <v>20</v>
+      </c>
+      <c r="F3">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -865,8 +889,14 @@
       <c r="D4" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>20</v>
+      </c>
+      <c r="F4">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -879,8 +909,14 @@
       <c r="D5" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>20</v>
+      </c>
+      <c r="F5">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -893,8 +929,14 @@
       <c r="D6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>20</v>
+      </c>
+      <c r="F6">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -907,8 +949,14 @@
       <c r="D7" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>20</v>
+      </c>
+      <c r="F7">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -921,8 +969,14 @@
       <c r="D8" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>20</v>
+      </c>
+      <c r="F8">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -935,8 +989,14 @@
       <c r="D9" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>20</v>
+      </c>
+      <c r="F9">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -949,8 +1009,14 @@
       <c r="D10" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>20</v>
+      </c>
+      <c r="F10">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -963,8 +1029,14 @@
       <c r="D11" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>20</v>
+      </c>
+      <c r="F11">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -977,8 +1049,14 @@
       <c r="D12" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>20</v>
+      </c>
+      <c r="F12">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -991,8 +1069,14 @@
       <c r="D13" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>20</v>
+      </c>
+      <c r="F13">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1005,8 +1089,14 @@
       <c r="D14" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>20</v>
+      </c>
+      <c r="F14">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1019,8 +1109,14 @@
       <c r="D15" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>20</v>
+      </c>
+      <c r="F15">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>15</v>
       </c>
@@ -1033,8 +1129,14 @@
       <c r="D16" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16">
+        <v>20</v>
+      </c>
+      <c r="F16">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>16</v>
       </c>
@@ -1047,8 +1149,14 @@
       <c r="D17" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17">
+        <v>20</v>
+      </c>
+      <c r="F17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>17</v>
       </c>
@@ -1061,8 +1169,14 @@
       <c r="D18" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>20</v>
+      </c>
+      <c r="F18">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>18</v>
       </c>
@@ -1075,8 +1189,14 @@
       <c r="D19" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19">
+        <v>20</v>
+      </c>
+      <c r="F19">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>19</v>
       </c>
@@ -1089,8 +1209,14 @@
       <c r="D20" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20">
+        <v>20</v>
+      </c>
+      <c r="F20">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>20</v>
       </c>
@@ -1103,8 +1229,14 @@
       <c r="D21" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21">
+        <v>20</v>
+      </c>
+      <c r="F21">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>21</v>
       </c>
@@ -1117,8 +1249,14 @@
       <c r="D22" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22">
+        <v>20</v>
+      </c>
+      <c r="F22">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>22</v>
       </c>
@@ -1131,8 +1269,14 @@
       <c r="D23" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23">
+        <v>20</v>
+      </c>
+      <c r="F23">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>23</v>
       </c>
@@ -1145,8 +1289,14 @@
       <c r="D24" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24">
+        <v>20</v>
+      </c>
+      <c r="F24">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>24</v>
       </c>
@@ -1159,8 +1309,14 @@
       <c r="D25" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25">
+        <v>20</v>
+      </c>
+      <c r="F25">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>25</v>
       </c>
@@ -1173,8 +1329,14 @@
       <c r="D26" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26">
+        <v>20</v>
+      </c>
+      <c r="F26">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>26</v>
       </c>
@@ -1187,8 +1349,14 @@
       <c r="D27" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27">
+        <v>20</v>
+      </c>
+      <c r="F27">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>27</v>
       </c>
@@ -1201,8 +1369,14 @@
       <c r="D28" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28">
+        <v>20</v>
+      </c>
+      <c r="F28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>28</v>
       </c>
@@ -1215,8 +1389,14 @@
       <c r="D29" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29">
+        <v>20</v>
+      </c>
+      <c r="F29">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>29</v>
       </c>
@@ -1229,8 +1409,14 @@
       <c r="D30" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E30">
+        <v>20</v>
+      </c>
+      <c r="F30">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>30</v>
       </c>
@@ -1243,8 +1429,14 @@
       <c r="D31" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E31">
+        <v>20</v>
+      </c>
+      <c r="F31">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>31</v>
       </c>
@@ -1257,8 +1449,14 @@
       <c r="D32" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E32">
+        <v>20</v>
+      </c>
+      <c r="F32">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>32</v>
       </c>
@@ -1271,8 +1469,14 @@
       <c r="D33" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E33">
+        <v>20</v>
+      </c>
+      <c r="F33">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>33</v>
       </c>
@@ -1285,8 +1489,14 @@
       <c r="D34" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E34">
+        <v>20</v>
+      </c>
+      <c r="F34">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>34</v>
       </c>
@@ -1299,8 +1509,14 @@
       <c r="D35" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E35">
+        <v>20</v>
+      </c>
+      <c r="F35">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>35</v>
       </c>
@@ -1313,8 +1529,14 @@
       <c r="D36" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E36">
+        <v>20</v>
+      </c>
+      <c r="F36">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>36</v>
       </c>
@@ -1327,8 +1549,14 @@
       <c r="D37" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E37">
+        <v>20</v>
+      </c>
+      <c r="F37">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>37</v>
       </c>
@@ -1341,8 +1569,14 @@
       <c r="D38" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E38">
+        <v>20</v>
+      </c>
+      <c r="F38">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>38</v>
       </c>
@@ -1355,8 +1589,14 @@
       <c r="D39" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E39">
+        <v>20</v>
+      </c>
+      <c r="F39">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>39</v>
       </c>
@@ -1369,8 +1609,14 @@
       <c r="D40" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E40">
+        <v>20</v>
+      </c>
+      <c r="F40">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>40</v>
       </c>
@@ -1383,8 +1629,14 @@
       <c r="D41" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E41">
+        <v>20</v>
+      </c>
+      <c r="F41">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>41</v>
       </c>
@@ -1397,8 +1649,14 @@
       <c r="D42" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E42">
+        <v>20</v>
+      </c>
+      <c r="F42">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>42</v>
       </c>
@@ -1411,8 +1669,14 @@
       <c r="D43" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E43">
+        <v>20</v>
+      </c>
+      <c r="F43">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>43</v>
       </c>
@@ -1425,8 +1689,14 @@
       <c r="D44" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E44">
+        <v>20</v>
+      </c>
+      <c r="F44">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>44</v>
       </c>
@@ -1439,8 +1709,14 @@
       <c r="D45" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E45">
+        <v>20</v>
+      </c>
+      <c r="F45">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>45</v>
       </c>
@@ -1453,8 +1729,14 @@
       <c r="D46" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E46">
+        <v>20</v>
+      </c>
+      <c r="F46">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>46</v>
       </c>
@@ -1467,8 +1749,14 @@
       <c r="D47" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E47">
+        <v>20</v>
+      </c>
+      <c r="F47">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>47</v>
       </c>
@@ -1481,8 +1769,14 @@
       <c r="D48" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E48">
+        <v>20</v>
+      </c>
+      <c r="F48">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>48</v>
       </c>
@@ -1495,8 +1789,14 @@
       <c r="D49" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E49">
+        <v>20</v>
+      </c>
+      <c r="F49">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>49</v>
       </c>
@@ -1509,8 +1809,14 @@
       <c r="D50" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E50">
+        <v>20</v>
+      </c>
+      <c r="F50">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>50</v>
       </c>
@@ -1523,8 +1829,14 @@
       <c r="D51" t="s">
         <v>104</v>
       </c>
-    </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E51">
+        <v>20</v>
+      </c>
+      <c r="F51">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>51</v>
       </c>
@@ -1537,8 +1849,14 @@
       <c r="D52" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E52">
+        <v>20</v>
+      </c>
+      <c r="F52">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>52</v>
       </c>
@@ -1551,8 +1869,14 @@
       <c r="D53" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E53">
+        <v>20</v>
+      </c>
+      <c r="F53">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>53</v>
       </c>
@@ -1565,8 +1889,14 @@
       <c r="D54" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E54">
+        <v>20</v>
+      </c>
+      <c r="F54">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>54</v>
       </c>
@@ -1579,8 +1909,14 @@
       <c r="D55" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E55">
+        <v>20</v>
+      </c>
+      <c r="F55">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>55</v>
       </c>
@@ -1593,8 +1929,14 @@
       <c r="D56" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E56">
+        <v>20</v>
+      </c>
+      <c r="F56">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>56</v>
       </c>
@@ -1607,8 +1949,14 @@
       <c r="D57" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E57">
+        <v>20</v>
+      </c>
+      <c r="F57">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>57</v>
       </c>
@@ -1621,8 +1969,14 @@
       <c r="D58" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E58">
+        <v>20</v>
+      </c>
+      <c r="F58">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>58</v>
       </c>
@@ -1635,8 +1989,14 @@
       <c r="D59" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E59">
+        <v>20</v>
+      </c>
+      <c r="F59">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>59</v>
       </c>
@@ -1649,8 +2009,14 @@
       <c r="D60" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E60">
+        <v>20</v>
+      </c>
+      <c r="F60">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>60</v>
       </c>
@@ -1663,8 +2029,14 @@
       <c r="D61" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E61">
+        <v>20</v>
+      </c>
+      <c r="F61">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>61</v>
       </c>
@@ -1677,8 +2049,14 @@
       <c r="D62" t="s">
         <v>127</v>
       </c>
-    </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E62">
+        <v>20</v>
+      </c>
+      <c r="F62">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>62</v>
       </c>
@@ -1691,8 +2069,14 @@
       <c r="D63" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E63">
+        <v>20</v>
+      </c>
+      <c r="F63">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>63</v>
       </c>
@@ -1705,8 +2089,14 @@
       <c r="D64" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E64">
+        <v>20</v>
+      </c>
+      <c r="F64">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="65" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>64</v>
       </c>
@@ -1719,8 +2109,14 @@
       <c r="D65" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E65">
+        <v>20</v>
+      </c>
+      <c r="F65">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="66" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>65</v>
       </c>
@@ -1733,8 +2129,14 @@
       <c r="D66" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E66">
+        <v>20</v>
+      </c>
+      <c r="F66">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="67" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>66</v>
       </c>
@@ -1747,8 +2149,14 @@
       <c r="D67" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E67">
+        <v>20</v>
+      </c>
+      <c r="F67">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="68" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>67</v>
       </c>
@@ -1761,8 +2169,14 @@
       <c r="D68" t="s">
         <v>25</v>
       </c>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E68">
+        <v>20</v>
+      </c>
+      <c r="F68">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="69" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>68</v>
       </c>
@@ -1775,8 +2189,14 @@
       <c r="D69" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E69">
+        <v>20</v>
+      </c>
+      <c r="F69">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="70" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>69</v>
       </c>
@@ -1789,8 +2209,14 @@
       <c r="D70" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E70">
+        <v>20</v>
+      </c>
+      <c r="F70">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="71" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>70</v>
       </c>
@@ -1802,6 +2228,12 @@
       </c>
       <c r="D71" t="s">
         <v>15</v>
+      </c>
+      <c r="E71">
+        <v>20</v>
+      </c>
+      <c r="F71">
+        <v>20</v>
       </c>
     </row>
   </sheetData>

</xml_diff>